<commit_message>
correction génération données fichiers json lorsque une données de l'étudiant n'existe pas dans la base de données(ues, semestre ou années de formation exécutée par l'étudiant) alors remplacée par la valeur NULL)
</commit_message>
<xml_diff>
--- a/projetS5/public/INFO/2018-2019/INFO1/S1/UE11/AP1.xlsx
+++ b/projetS5/public/INFO/2018-2019/INFO1/S1/UE11/AP1.xlsx
@@ -732,7 +732,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>20150926</v>
+        <v>20170926</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -744,12 +744,12 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>20150927</v>
+        <v>20170927</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -761,12 +761,12 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>20150928</v>
+        <v>20170928</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -778,12 +778,12 @@
         <v>14</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>20150929</v>
+        <v>20170929</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -795,12 +795,12 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>20150930</v>
+        <v>20170930</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -812,12 +812,12 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>20150931</v>
+        <v>20170931</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -829,12 +829,12 @@
         <v>8</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>20150932</v>
+        <v>20170932</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -846,12 +846,12 @@
         <v>11</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>20150933</v>
+        <v>20170933</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -863,12 +863,12 @@
         <v>11</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>20150934</v>
+        <v>20170934</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -880,12 +880,12 @@
         <v>8</v>
       </c>
       <c r="E11">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>20150935</v>
+        <v>20170935</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
@@ -897,12 +897,12 @@
         <v>11</v>
       </c>
       <c r="E12">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>20150936</v>
+        <v>20170936</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
@@ -914,12 +914,12 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>20150937</v>
+        <v>20170937</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -931,12 +931,12 @@
         <v>11</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>20150938</v>
+        <v>20170938</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -948,12 +948,12 @@
         <v>8</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>20150939</v>
+        <v>20170939</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -965,12 +965,12 @@
         <v>14</v>
       </c>
       <c r="E16">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>20150940</v>
+        <v>20170940</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -982,12 +982,12 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>20150941</v>
+        <v>20170941</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
@@ -999,12 +999,12 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>20150942</v>
+        <v>20170942</v>
       </c>
       <c r="B19" t="s">
         <v>39</v>
@@ -1016,12 +1016,12 @@
         <v>8</v>
       </c>
       <c r="E19">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>20150943</v>
+        <v>20170943</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
@@ -1033,12 +1033,12 @@
         <v>8</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>20150944</v>
+        <v>20170944</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -1050,12 +1050,12 @@
         <v>8</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>20150945</v>
+        <v>20170945</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
@@ -1067,12 +1067,12 @@
         <v>11</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>20150946</v>
+        <v>20170946</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -1084,12 +1084,12 @@
         <v>14</v>
       </c>
       <c r="E23">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>20150947</v>
+        <v>20170947</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -1101,12 +1101,12 @@
         <v>14</v>
       </c>
       <c r="E24">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>20150948</v>
+        <v>20170948</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
@@ -1118,12 +1118,12 @@
         <v>8</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>20150949</v>
+        <v>20170949</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
@@ -1135,12 +1135,12 @@
         <v>8</v>
       </c>
       <c r="E26">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>20150950</v>
+        <v>20170950</v>
       </c>
       <c r="B27" t="s">
         <v>54</v>
@@ -1152,12 +1152,12 @@
         <v>14</v>
       </c>
       <c r="E27">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>20150951</v>
+        <v>20170951</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
@@ -1169,12 +1169,12 @@
         <v>11</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>20150952</v>
+        <v>20170952</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
@@ -1186,12 +1186,12 @@
         <v>8</v>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>20150953</v>
+        <v>20170953</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
@@ -1203,12 +1203,12 @@
         <v>8</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>20150954</v>
+        <v>20170954</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
@@ -1220,12 +1220,12 @@
         <v>14</v>
       </c>
       <c r="E31">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>20150955</v>
+        <v>20170955</v>
       </c>
       <c r="B32" t="s">
         <v>61</v>
@@ -1237,12 +1237,12 @@
         <v>11</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>20150956</v>
+        <v>20170956</v>
       </c>
       <c r="B33" t="s">
         <v>63</v>
@@ -1254,12 +1254,12 @@
         <v>8</v>
       </c>
       <c r="E33">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>20150957</v>
+        <v>20170957</v>
       </c>
       <c r="B34" t="s">
         <v>65</v>
@@ -1271,12 +1271,12 @@
         <v>11</v>
       </c>
       <c r="E34">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>20150958</v>
+        <v>20170958</v>
       </c>
       <c r="B35" t="s">
         <v>67</v>
@@ -1288,12 +1288,12 @@
         <v>14</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>20150959</v>
+        <v>20170959</v>
       </c>
       <c r="B36" t="s">
         <v>68</v>
@@ -1305,12 +1305,12 @@
         <v>11</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>20150960</v>
+        <v>20170960</v>
       </c>
       <c r="B37" t="s">
         <v>70</v>
@@ -1322,12 +1322,12 @@
         <v>14</v>
       </c>
       <c r="E37">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>20150961</v>
+        <v>20170961</v>
       </c>
       <c r="B38" t="s">
         <v>72</v>
@@ -1339,12 +1339,12 @@
         <v>14</v>
       </c>
       <c r="E38">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>20150962</v>
+        <v>20170962</v>
       </c>
       <c r="B39" t="s">
         <v>74</v>
@@ -1356,12 +1356,12 @@
         <v>14</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>20150963</v>
+        <v>20170963</v>
       </c>
       <c r="B40" t="s">
         <v>75</v>
@@ -1373,12 +1373,12 @@
         <v>8</v>
       </c>
       <c r="E40">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>20150964</v>
+        <v>20170964</v>
       </c>
       <c r="B41" t="s">
         <v>77</v>
@@ -1390,12 +1390,12 @@
         <v>14</v>
       </c>
       <c r="E41">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>20150965</v>
+        <v>20170965</v>
       </c>
       <c r="B42" t="s">
         <v>78</v>
@@ -1407,12 +1407,12 @@
         <v>11</v>
       </c>
       <c r="E42">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>20150966</v>
+        <v>20170966</v>
       </c>
       <c r="B43" t="s">
         <v>80</v>
@@ -1424,12 +1424,12 @@
         <v>14</v>
       </c>
       <c r="E43">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>20150967</v>
+        <v>20170967</v>
       </c>
       <c r="B44" t="s">
         <v>81</v>
@@ -1441,12 +1441,12 @@
         <v>14</v>
       </c>
       <c r="E44">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>20150968</v>
+        <v>20170968</v>
       </c>
       <c r="B45" t="s">
         <v>83</v>
@@ -1458,12 +1458,12 @@
         <v>11</v>
       </c>
       <c r="E45">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>20150969</v>
+        <v>20170969</v>
       </c>
       <c r="B46" t="s">
         <v>85</v>
@@ -1475,12 +1475,12 @@
         <v>14</v>
       </c>
       <c r="E46">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>20150970</v>
+        <v>20170970</v>
       </c>
       <c r="B47" t="s">
         <v>86</v>
@@ -1492,12 +1492,12 @@
         <v>8</v>
       </c>
       <c r="E47">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>20150971</v>
+        <v>20170971</v>
       </c>
       <c r="B48" t="s">
         <v>88</v>
@@ -1509,12 +1509,12 @@
         <v>11</v>
       </c>
       <c r="E48">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>20150972</v>
+        <v>20170972</v>
       </c>
       <c r="B49" t="s">
         <v>90</v>
@@ -1526,12 +1526,12 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>20150973</v>
+        <v>20170973</v>
       </c>
       <c r="B50" t="s">
         <v>92</v>
@@ -1543,12 +1543,12 @@
         <v>8</v>
       </c>
       <c r="E50">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>20150974</v>
+        <v>20170974</v>
       </c>
       <c r="B51" t="s">
         <v>93</v>
@@ -1560,12 +1560,12 @@
         <v>11</v>
       </c>
       <c r="E51">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>20150975</v>
+        <v>20170975</v>
       </c>
       <c r="B52" t="s">
         <v>95</v>
@@ -1577,12 +1577,12 @@
         <v>14</v>
       </c>
       <c r="E52">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>20150976</v>
+        <v>20170976</v>
       </c>
       <c r="B53" t="s">
         <v>96</v>
@@ -1594,12 +1594,12 @@
         <v>8</v>
       </c>
       <c r="E53">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>20150977</v>
+        <v>20170977</v>
       </c>
       <c r="B54" t="s">
         <v>98</v>
@@ -1611,12 +1611,12 @@
         <v>11</v>
       </c>
       <c r="E54">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>20150978</v>
+        <v>20170978</v>
       </c>
       <c r="B55" t="s">
         <v>99</v>
@@ -1628,12 +1628,12 @@
         <v>11</v>
       </c>
       <c r="E55">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>20150979</v>
+        <v>20170979</v>
       </c>
       <c r="B56" t="s">
         <v>101</v>
@@ -1645,12 +1645,12 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>20150980</v>
+        <v>20170980</v>
       </c>
       <c r="B57" t="s">
         <v>102</v>
@@ -1662,12 +1662,12 @@
         <v>14</v>
       </c>
       <c r="E57">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>20150981</v>
+        <v>20170981</v>
       </c>
       <c r="B58" t="s">
         <v>104</v>
@@ -1679,12 +1679,12 @@
         <v>8</v>
       </c>
       <c r="E58">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>20150982</v>
+        <v>20170982</v>
       </c>
       <c r="B59" t="s">
         <v>105</v>
@@ -1696,12 +1696,12 @@
         <v>8</v>
       </c>
       <c r="E59">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>20150983</v>
+        <v>20170983</v>
       </c>
       <c r="B60" t="s">
         <v>107</v>
@@ -1713,12 +1713,12 @@
         <v>14</v>
       </c>
       <c r="E60">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>20150984</v>
+        <v>20170984</v>
       </c>
       <c r="B61" t="s">
         <v>108</v>
@@ -1730,12 +1730,12 @@
         <v>11</v>
       </c>
       <c r="E61">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>20150985</v>
+        <v>20170985</v>
       </c>
       <c r="B62" t="s">
         <v>110</v>
@@ -1747,12 +1747,12 @@
         <v>14</v>
       </c>
       <c r="E62">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>20150986</v>
+        <v>20170986</v>
       </c>
       <c r="B63" t="s">
         <v>112</v>
@@ -1764,7 +1764,7 @@
         <v>8</v>
       </c>
       <c r="E63">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>